<commit_message>
all feature xls added
</commit_message>
<xml_diff>
--- a/Stylogenetics/my_main_data/#Cosine Similarity[.]/result analysis/Feature wise result.xlsx
+++ b/Stylogenetics/my_main_data/#Cosine Similarity[.]/result analysis/Feature wise result.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tahmidolee\Dropbox\SHARED (1)\OLEE&amp;MMRS\Project 300\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tahmidolee\Documents\Project 300\Stylogenetics\Stylogenetics\my_main_data\#Cosine Similarity[.]\result analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,6 +21,40 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Tahmidolee</author>
+  </authors>
+  <commentList>
+    <comment ref="D6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tahmidolee:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -63,13 +97,26 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -92,8 +139,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -125,40 +173,19 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="8.384693819747352E-2"/>
+          <c:y val="0.18065841449945688"/>
+          <c:w val="0.88977416492003247"/>
+          <c:h val="0.60640874246942733"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -217,25 +244,25 @@
             <c:numRef>
               <c:f>Sheet1!$B$2:$G$2</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>86</c:v>
+                  <c:v>0.86</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>98</c:v>
+                  <c:v>0.98</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>66</c:v>
+                  <c:v>0.66</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>96</c:v>
+                  <c:v>0.96</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>96</c:v>
+                  <c:v>0.96</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>100</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -295,25 +322,25 @@
             <c:numRef>
               <c:f>Sheet1!$B$3:$G$3</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>96</c:v>
+                  <c:v>0.96</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>98</c:v>
+                  <c:v>0.98</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>52</c:v>
+                  <c:v>0.52</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>98</c:v>
+                  <c:v>0.98</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>98</c:v>
+                  <c:v>0.98</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>98</c:v>
+                  <c:v>0.98</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -373,25 +400,25 @@
             <c:numRef>
               <c:f>Sheet1!$B$4:$G$4</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>94</c:v>
+                  <c:v>0.94</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>96</c:v>
+                  <c:v>0.96</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>46</c:v>
+                  <c:v>0.46</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>96</c:v>
+                  <c:v>0.96</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>98</c:v>
+                  <c:v>0.98</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>98</c:v>
+                  <c:v>0.98</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -451,25 +478,25 @@
             <c:numRef>
               <c:f>Sheet1!$B$5:$G$5</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>98</c:v>
+                  <c:v>0.98</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>84</c:v>
+                  <c:v>0.84</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>54</c:v>
+                  <c:v>0.54</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>88</c:v>
+                  <c:v>0.88</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>82</c:v>
+                  <c:v>0.82</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>80</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -529,25 +556,25 @@
             <c:numRef>
               <c:f>Sheet1!$B$6:$G$6</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>64</c:v>
+                  <c:v>0.64</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>88</c:v>
+                  <c:v>0.88</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>66</c:v>
+                  <c:v>0.66</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>98</c:v>
+                  <c:v>0.98</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>84</c:v>
+                  <c:v>0.84</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>100</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -563,11 +590,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="109144976"/>
-        <c:axId val="109122192"/>
+        <c:axId val="110489232"/>
+        <c:axId val="110671088"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="109144976"/>
+        <c:axId val="110489232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -610,7 +637,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="109122192"/>
+        <c:crossAx val="110671088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -618,9 +645,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="109122192"/>
+        <c:axId val="110671088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -638,7 +666,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -669,7 +697,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="109144976"/>
+        <c:crossAx val="110489232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -745,7 +773,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -1297,16 +1325,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>371474</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>185736</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1276348</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>128583</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>285749</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>114299</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>85724</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1590,11 +1618,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1626,119 +1654,121 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>86</v>
-      </c>
-      <c r="C2">
-        <v>98</v>
-      </c>
-      <c r="D2">
-        <v>66</v>
-      </c>
-      <c r="E2">
-        <v>96</v>
-      </c>
-      <c r="F2">
-        <v>96</v>
-      </c>
-      <c r="G2">
-        <v>100</v>
+      <c r="B2" s="1">
+        <v>0.86</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.98</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.66</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.96</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.96</v>
+      </c>
+      <c r="G2" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>96</v>
-      </c>
-      <c r="C3">
-        <v>98</v>
-      </c>
-      <c r="D3">
-        <v>52</v>
-      </c>
-      <c r="E3">
-        <v>98</v>
-      </c>
-      <c r="F3">
-        <v>98</v>
-      </c>
-      <c r="G3">
-        <v>98</v>
+      <c r="B3" s="1">
+        <v>0.96</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.98</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.52</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.98</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.98</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0.98</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
-        <v>94</v>
-      </c>
-      <c r="C4">
-        <v>96</v>
-      </c>
-      <c r="D4">
-        <v>46</v>
-      </c>
-      <c r="E4">
-        <v>96</v>
-      </c>
-      <c r="F4">
-        <v>98</v>
-      </c>
-      <c r="G4">
-        <v>98</v>
+      <c r="B4" s="1">
+        <v>0.94</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.96</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.46</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.96</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.98</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.98</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5">
-        <v>98</v>
-      </c>
-      <c r="C5">
-        <v>84</v>
-      </c>
-      <c r="D5">
-        <v>54</v>
-      </c>
-      <c r="E5">
-        <v>88</v>
-      </c>
-      <c r="F5">
-        <v>82</v>
-      </c>
-      <c r="G5">
-        <v>80</v>
+      <c r="B5" s="1">
+        <v>0.98</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.84</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.54</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.82</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.8</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6">
-        <v>64</v>
-      </c>
-      <c r="C6">
-        <v>88</v>
-      </c>
-      <c r="D6">
-        <v>66</v>
-      </c>
-      <c r="E6">
-        <v>98</v>
-      </c>
-      <c r="F6">
-        <v>84</v>
-      </c>
-      <c r="G6">
-        <v>100</v>
+      <c r="B6" s="1">
+        <v>0.64</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.66</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.98</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0.84</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>